<commit_message>
Updated the notebook with corrections to objective function
</commit_message>
<xml_diff>
--- a/Predictions of Optimization Loop 1.xlsx
+++ b/Predictions of Optimization Loop 1.xlsx
@@ -525,13 +525,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>18.25</v>
+        <v>86.31999969482422</v>
       </c>
       <c r="C2" t="n">
-        <v>96.76999664306641</v>
+        <v>81.62000274658203</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.690000057220459</v>
+        <v>-1.450000047683716</v>
       </c>
       <c r="E2" t="n">
         <v>51.54999923706055</v>
@@ -540,16 +540,16 @@
         <v>8.44</v>
       </c>
       <c r="G2" t="n">
-        <v>6.110000133514404</v>
+        <v>5.639999866485596</v>
       </c>
       <c r="H2" t="n">
-        <v>3.99</v>
+        <v>4</v>
       </c>
       <c r="I2" t="n">
-        <v>3.890000104904175</v>
+        <v>3.849999904632568</v>
       </c>
       <c r="J2" t="n">
-        <v>3.33</v>
+        <v>3.34</v>
       </c>
       <c r="K2" t="n">
         <v>7.880000114440918</v>
@@ -558,22 +558,22 @@
         <v>4.25</v>
       </c>
       <c r="M2" t="n">
-        <v>25.71999931335449</v>
+        <v>26.36000061035156</v>
       </c>
       <c r="N2" t="n">
-        <v>10.62</v>
+        <v>10.67</v>
       </c>
       <c r="O2" t="n">
-        <v>2.519999980926514</v>
+        <v>2.5</v>
       </c>
       <c r="P2" t="n">
-        <v>2.4</v>
+        <v>2.42</v>
       </c>
       <c r="Q2" t="n">
-        <v>-320.9599914550781</v>
+        <v>-322.25</v>
       </c>
       <c r="R2" t="n">
-        <v>71.51000000000001</v>
+        <v>72.54000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -581,55 +581,55 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>43.45999908447266</v>
+        <v>22.80999946594238</v>
       </c>
       <c r="C3" t="n">
-        <v>56.84999847412109</v>
+        <v>24.72999954223633</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.580000042915344</v>
+        <v>-1.639999985694885</v>
       </c>
       <c r="E3" t="n">
-        <v>47.81000137329102</v>
+        <v>53.11999893188477</v>
       </c>
       <c r="F3" t="n">
-        <v>7.39</v>
+        <v>7.73</v>
       </c>
       <c r="G3" t="n">
-        <v>2.700000047683716</v>
+        <v>4.110000133514404</v>
       </c>
       <c r="H3" t="n">
-        <v>3.33</v>
+        <v>3.8</v>
       </c>
       <c r="I3" t="n">
-        <v>1.440000057220459</v>
+        <v>2.210000038146973</v>
       </c>
       <c r="J3" t="n">
-        <v>2.56</v>
+        <v>2.39</v>
       </c>
       <c r="K3" t="n">
-        <v>4.440000057220459</v>
+        <v>6.230000019073486</v>
       </c>
       <c r="L3" t="n">
-        <v>3.37</v>
+        <v>3.12</v>
       </c>
       <c r="M3" t="n">
-        <v>45.40000152587891</v>
+        <v>32.04999923706055</v>
       </c>
       <c r="N3" t="n">
-        <v>6.35</v>
+        <v>5.81</v>
       </c>
       <c r="O3" t="n">
-        <v>0.949999988079071</v>
+        <v>1.25</v>
       </c>
       <c r="P3" t="n">
-        <v>2.03</v>
+        <v>1.81</v>
       </c>
       <c r="Q3" t="n">
-        <v>-378.4500122070312</v>
+        <v>-338.3099975585938</v>
       </c>
       <c r="R3" t="n">
-        <v>70.52</v>
+        <v>74.48999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -637,55 +637,55 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>18.69000053405762</v>
+        <v>97.87999725341797</v>
       </c>
       <c r="C4" t="n">
-        <v>70.73000335693359</v>
+        <v>73.70999908447266</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.509999990463257</v>
+        <v>-1.450000047683716</v>
       </c>
       <c r="E4" t="n">
-        <v>50.52000045776367</v>
+        <v>51.54999923706055</v>
       </c>
       <c r="F4" t="n">
-        <v>8.41</v>
+        <v>8.44</v>
       </c>
       <c r="G4" t="n">
-        <v>4.239999771118164</v>
+        <v>5.650000095367432</v>
       </c>
       <c r="H4" t="n">
-        <v>3.57</v>
+        <v>4</v>
       </c>
       <c r="I4" t="n">
-        <v>2.720000028610229</v>
+        <v>3.849999904632568</v>
       </c>
       <c r="J4" t="n">
-        <v>2.97</v>
+        <v>3.34</v>
       </c>
       <c r="K4" t="n">
-        <v>7.199999809265137</v>
+        <v>7.880000114440918</v>
       </c>
       <c r="L4" t="n">
-        <v>4.09</v>
+        <v>4.25</v>
       </c>
       <c r="M4" t="n">
-        <v>36.25</v>
+        <v>26.27000045776367</v>
       </c>
       <c r="N4" t="n">
-        <v>9.23</v>
+        <v>10.67</v>
       </c>
       <c r="O4" t="n">
-        <v>1.970000028610229</v>
+        <v>2.5</v>
       </c>
       <c r="P4" t="n">
-        <v>1.96</v>
+        <v>2.42</v>
       </c>
       <c r="Q4" t="n">
-        <v>-333.7999877929688</v>
+        <v>-322.1799926757812</v>
       </c>
       <c r="R4" t="n">
-        <v>74.58</v>
+        <v>72.48999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -693,55 +693,55 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20.40999984741211</v>
+        <v>30.48999977111816</v>
       </c>
       <c r="C5" t="n">
-        <v>53.29999923706055</v>
+        <v>24.94000053405762</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.590000033378601</v>
+        <v>-1.549999952316284</v>
       </c>
       <c r="E5" t="n">
-        <v>52.61999893188477</v>
+        <v>48.91999816894531</v>
       </c>
       <c r="F5" t="n">
-        <v>4.55</v>
+        <v>7.99</v>
       </c>
       <c r="G5" t="n">
-        <v>0.8299999833106995</v>
+        <v>3.609999895095825</v>
       </c>
       <c r="H5" t="n">
-        <v>1.81</v>
+        <v>3.9</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8399999737739563</v>
+        <v>0.5400000214576721</v>
       </c>
       <c r="J5" t="n">
-        <v>1.33</v>
+        <v>2.12</v>
       </c>
       <c r="K5" t="n">
-        <v>4.639999866485596</v>
+        <v>3.390000104904175</v>
       </c>
       <c r="L5" t="n">
-        <v>2.31</v>
+        <v>3.05</v>
       </c>
       <c r="M5" t="n">
-        <v>39.36000061035156</v>
+        <v>49.27999877929688</v>
       </c>
       <c r="N5" t="n">
-        <v>4.75</v>
+        <v>6.09</v>
       </c>
       <c r="O5" t="n">
-        <v>0.2000000029802322</v>
+        <v>0.6399999856948853</v>
       </c>
       <c r="P5" t="n">
-        <v>0.63</v>
+        <v>0.83</v>
       </c>
       <c r="Q5" t="n">
-        <v>-323.6900024414062</v>
+        <v>-356.4200134277344</v>
       </c>
       <c r="R5" t="n">
-        <v>59.08</v>
+        <v>73.59</v>
       </c>
     </row>
     <row r="6">
@@ -749,55 +749,55 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>47.06000137329102</v>
+        <v>80.81999969482422</v>
       </c>
       <c r="C6" t="n">
-        <v>61.36000061035156</v>
+        <v>14.15999984741211</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.590000033378601</v>
+        <v>-1.580000042915344</v>
       </c>
       <c r="E6" t="n">
-        <v>49.02999877929688</v>
+        <v>51.61999893188477</v>
       </c>
       <c r="F6" t="n">
-        <v>7.83</v>
+        <v>8.44</v>
       </c>
       <c r="G6" t="n">
-        <v>2.150000095367432</v>
+        <v>5.269999980926514</v>
       </c>
       <c r="H6" t="n">
-        <v>2.88</v>
+        <v>3.98</v>
       </c>
       <c r="I6" t="n">
-        <v>1.519999980926514</v>
+        <v>3.849999904632568</v>
       </c>
       <c r="J6" t="n">
-        <v>2.61</v>
+        <v>3.34</v>
       </c>
       <c r="K6" t="n">
-        <v>4.550000190734863</v>
+        <v>7.869999885559082</v>
       </c>
       <c r="L6" t="n">
-        <v>3.61</v>
+        <v>4.25</v>
       </c>
       <c r="M6" t="n">
-        <v>42.58000183105469</v>
+        <v>27.03000068664551</v>
       </c>
       <c r="N6" t="n">
-        <v>7.24</v>
+        <v>10.62</v>
       </c>
       <c r="O6" t="n">
-        <v>0.9599999785423279</v>
+        <v>2.5</v>
       </c>
       <c r="P6" t="n">
-        <v>1.98</v>
+        <v>2.42</v>
       </c>
       <c r="Q6" t="n">
-        <v>-384.3099975585938</v>
+        <v>-323.5</v>
       </c>
       <c r="R6" t="n">
-        <v>69.20999999999999</v>
+        <v>73.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>